<commit_message>
Attaching race data to new figures
</commit_message>
<xml_diff>
--- a/fallClean/RaceInfo/fa_info_fri.xlsx
+++ b/fallClean/RaceInfo/fa_info_fri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabby/Desktop/dragraceAnalysis-master/fallClean/RaceInfo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabby/Library/Containers/com.microsoft.Excel/Data/Desktop/dragraceAnalysis-master/fallClean/RaceInfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CFB4EA-5FF6-D047-8737-283DB27F2137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5003D73-8431-2C4E-ADF4-EEBDE6BB6BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="2960" windowWidth="26040" windowHeight="13820" xr2:uid="{88E1B4FB-5D42-DC41-9834-5B803F3034D3}"/>
   </bookViews>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2817F70-CBF0-4E43-87CD-DF3EB643CB4F}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>